<commit_message>
add prompt about date which shuld have space
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F476"/>
+  <dimension ref="A1:F497"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44778,6 +44778,1904 @@
         </is>
       </c>
     </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>世建发票1.pdf</t>
+        </is>
+      </c>
+      <c r="B477" t="n">
+        <v>1</v>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827520",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 12474.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827520",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 12474.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世世世世(香香)有有有有 InvoiceNo. :90827520
+Currency :USD
+IssuedBy :VickyYan
+Salesman :TONYGUO
+Date :28Aug2023
+Customer Code :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK)
+COLIMITED COLIMITED
+ROOMS3101-3105SINGGACOMMERCIALCENTRE ROOMS3101-3105SINGGACOMMERCIALCENTRE
+148CONNAUGHT ROADWEST 148CONNAUGHT ROADWEST
+WESTERN DISTRICT,Hong Kong WESTERN DISTRICT,Hong Kong
+海海海海海海海海海(香香)有有有有 海海海海海海海海海(香香)有有有有
+Tel:852-25935622 Tel:852-25935622
+____________________________________________________________________________________________________
+TERMS OFPAYMENT:60DAYSAMS
+TERMS OFSHIPMENT: FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTY Unit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0200 ADP2120ACPZ-R7 4510066029 31,500PC 0.396000 12,474.00
+______3_0_1_00_7_8_4_01________________8_0_7_9_70_9_7__________________________________________________________________
+Total: 31,500PC 12,474.00
+LessDepositPaid: 0.00
+NetTotal: 12,474.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出出出出出出(編編EN-1102)isattached
+INV#90827520,BRAND:ADI,COUNTRYOFORIGIN:SOUTHKOREA
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39Wang KwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>世建发票1.pdf</t>
+        </is>
+      </c>
+      <c r="B478" t="n">
+        <v>2</v>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827622",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 7155.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827622",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 7155.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世世世世(香香)有有有有 InvoiceNo. :90827622
+Currency :USD
+IssuedBy :VickyYan
+Salesman :TONYGUO
+Date :28Aug2023
+Customer Code :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK)
+COLIMITED COLIMITED
+ROOMS3101-3105SINGGACOMMERCIALCENTRE ROOMS3101-3105SINGGACOMMERCIALCENTRE
+148CONNAUGHT ROADWEST 148CONNAUGHT ROADWEST
+WESTERN DISTRICT,Hong Kong WESTERN DISTRICT,Hong Kong
+海海海海海海海海海(香香)有有有有 海海海海海海海海海(香香)有有有有
+Tel:852-25935622 Tel:852-25935622
+____________________________________________________________________________________________________
+TERMS OFPAYMENT:60DAYSAMS
+TERMS OFSHIPMENT: FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTY Unit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0010 ADUCM420BCBZ-RL7 4510079885 1,500PC 4.770000 7,155.00
+______3_0_1_11_0_6_1_01________________8_0_7_9_71_9_4__________________________________________________________________
+Total: 1,500PC 7,155.00
+LessDepositPaid: 0.00
+NetTotal: 7,155.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出出出出出出(編編EN-1102)isattached
+INV#90827622,BRAND:ADI,COUNTRYOFORIGIN: SINGAPORE
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39Wang KwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>世建发票1.pdf</t>
+        </is>
+      </c>
+      <c r="B479" t="n">
+        <v>3</v>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827668",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 7155.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827668",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 7155.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世世世世(香香)有有有有 InvoiceNo. :90827668
+Currency :USD
+IssuedBy :VickyYan
+Salesman :TONYGUO
+Date :28Aug2023
+Customer Code :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK)
+COLIMITED COLIMITED
+ROOMS3101-3105SINGGACOMMERCIALCENTRE ROOMS3101-3105SINGGACOMMERCIALCENTRE
+148CONNAUGHT ROADWEST 148CONNAUGHT ROADWEST
+WESTERN DISTRICT,Hong Kong WESTERN DISTRICT,Hong Kong
+海海海海海海海海海(香香)有有有有 海海海海海海海海海(香香)有有有有
+Tel:852-25935622 Tel:852-25935622
+____________________________________________________________________________________________________
+TERMS OFPAYMENT:60DAYSAMS
+TERMS OFSHIPMENT: FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTY Unit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0010 ADUCM420BCBZ-RL7 4510080078 1,500PC 4.770000 7,155.00
+______3_0_1_11_0_6_1_01________________8_0_7_9_71_9_2__________________________________________________________________
+Total: 1,500PC 7,155.00
+LessDepositPaid: 0.00
+NetTotal: 7,155.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出出出出出出(編編EN-1102)isattached
+INV#90827668,BRAND:ADI,COUNTRYOFORIGIN:SINGAPORE
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39Wang KwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>世建发票1.pdf</t>
+        </is>
+      </c>
+      <c r="B480" t="n">
+        <v>4</v>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827701",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 23836.5,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90827701",
+    "Invoice Date": "28 Aug 2023",
+    "Currency": "USD",
+    "Amount": 23836.5,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世世世世(香香)有有有有 InvoiceNo. :90827701
+Currency :USD
+IssuedBy :VickyYan
+Salesman :TONYGUO
+Date :28Aug2023
+Customer Code :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK)
+COLIMITED COLIMITED
+ROOMS3101-3105SINGGACOMMERCIALCENTRE ROOMS3101-3105SINGGACOMMERCIALCENTRE
+148CONNAUGHT ROADWEST 148CONNAUGHT ROADWEST
+WESTERN DISTRICT,Hong Kong WESTERN DISTRICT,Hong Kong
+海海海海海海海海海(香香)有有有有 海海海海海海海海海(香香)有有有有
+Tel:852-25935622 Tel:852-25935622
+____________________________________________________________________________________________________
+TERMS OFPAYMENT:60DAYSAMS
+TERMS OFSHIPMENT: FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTY Unit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0010 ADUCM420BCBZ-RL7 4510077212 1,500PC 5.297000 7,945.50
+______3_0_1_11_0_6_1_01________________8_0_7_9_72_6_6__________________________________________________________________
+0070 ADUCM420BCBZ-RL7 4510077212 1,500PC 5.297000 7,945.50
+______3_0_1_11_0_6_1_01________________8_0_7_9_72_6_6__________________________________________________________________
+0100 ADUCM420BCBZ-RL7 4510077212 1,500PC 5.297000 7,945.50
+______3_0_1_11_0_6_1_01________________8_0_7_9_72_6_6__________________________________________________________________
+Total: 4,500PC 23,836.50
+LessDepositPaid: 0.00
+NetTotal: 23,836.50
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出出出出出出(編編EN-1102)isattached
+INV#90827701,BRAND:ADI,COUNTRYOFORIGIN:SINGAPORE
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39Wang KwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>世建发票7.pdf</t>
+        </is>
+      </c>
+      <c r="B481" t="n">
+        <v>1</v>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90817165",
+    "Invoice Date": "03Jul2023",
+    "Currency": "USD",
+    "Amount": 31782.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90817165",
+    "Invoice Date": "03Jul2023",
+    "Currency": "USD",
+    "Amount": 31782.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世世世世(香香)有有有有 InvoiceNo. :90817165
+Currency :USD
+IssuedBy :VickyYan
+Salesman :TONYGUO
+Date :03Jul2023
+Customer Code :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK)
+COLIMITED COLIMITED
+ROOMS3101-3105SINGGACOMMERCIALCENTRE ROOMS3101-3105SINGGACOMMERCIALCENTRE
+148CONNAUGHT ROADWEST 148CONNAUGHT ROADWEST
+WESTERN DISTRICT,Hong Kong WESTERN DISTRICT,Hong Kong
+海海海海海海海海海(香香)有有有有 海海海海海海海海海(香香)有有有有
+Tel:852-25935622 Tel:852-25935622
+____________________________________________________________________________________________________
+TERMS OFPAYMENT:60DAYSAMS
+TERMS OFSHIPMENT: FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTY Unit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0030 ADUCM420BCBZ-RL7 4510077212 1,500PC 5.297000 7,945.50
+______3_0_1_11_0_6_1_01________________8_0_7_8_69_5_8__________________________________________________________________
+0040 ADUCM420BCBZ-RL7 4510077212 1,500PC 5.297000 7,945.50
+______3_0_1_11_0_6_1_01________________8_0_7_8_69_5_8__________________________________________________________________
+0050 ADUCM420BCBZ-RL7 4510077212 1,500PC 5.297000 7,945.50
+______3_0_1_11_0_6_1_01________________8_0_7_8_69_5_8__________________________________________________________________
+0060 ADUCM420BCBZ-RL7 4510077212 1,500PC 5.297000 7,945.50
+______3_0_1_11_0_6_1_01________________8_0_7_8_69_5_8__________________________________________________________________
+Total: 6,000PC 31,782.00
+LessDepositPaid: 0.00
+NetTotal: 31,782.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出出出出出出(編編EN-1102)isattached
+INV#90817165,BRAND:ADI,COUNTRYOFORIGIN: SINGAPORE
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39Wang KwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>世建发票3.pdf</t>
+        </is>
+      </c>
+      <c r="B482" t="n">
+        <v>1</v>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824620",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 4750.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824620",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 4750.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世健系統(香港)有限公司 InvoiceNo. :90824620
+Currency :USD
+IssuedBy :ShirleyHu
+Salesman :TONYGUO
+Date :09Aug2023
+CustomerCode :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIESCO
+COLIMITED LTD
+ROOMS3101-3105SINGGACOMMERCIALCENTRE NO218QIANWANROAD
+148CONNAUGHTROADWEST QINGDAOECONOMICANDTECHNOLOGICAL
+WESTERNDISTRICT,HongKong DEVELOPMENTZONE
+海信寬帶多媒體技術(香港)有限公司 QINGDAO
+Tel:852-25935622 QINGDAO,China
+PostalCode:266071
+青島海信寬帶多媒體技術有限公司
+青島經濟技術開發區前灣路218號
+Tel:86-532-86016016Fax:86-532-86016007
+____________________________________________________________________________________________________
+TERMSOFPAYMENT:60DAYSAMS
+TERMSOFSHIPMENT:FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTYUnit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0370 ADUC7020BCPZ62I-RL 4570065409 2,500PC 1.900000 4,750.00
+______3_0_1_00_0_3_4_01________________8_0_7_9_42_9_1__________________________________________________________________
+Total: 2,500PC 4,750.00
+LessDepositPaid: 0.00
+NetTotal: 4,750.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出口事宜須知(編號EN-1102)isattached
+REF#AL0000036780,INV#90824620,BRAND:ADI,COUNTRYOFORIGIN:CHINA
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39WangKwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>世建发票3.pdf</t>
+        </is>
+      </c>
+      <c r="B483" t="n">
+        <v>2</v>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824626",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 4338.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824626",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 4338.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世健系統(香港)有限公司 InvoiceNo. :90824626
+Currency :USD
+IssuedBy :ShirleyHu
+Salesman :TONYGUO
+Date :09Aug2023
+CustomerCode :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIESCO
+COLIMITED LTD
+ROOMS3101-3105SINGGACOMMERCIALCENTRE NO218QIANWANROAD
+148CONNAUGHTROADWEST QINGDAOECONOMICANDTECHNOLOGICAL
+WESTERNDISTRICT,HongKong DEVELOPMENTZONE
+海信寬帶多媒體技術(香港)有限公司 QINGDAO
+Tel:852-25935622 QINGDAO,China
+PostalCode:266071
+青島海信寬帶多媒體技術有限公司
+青島經濟技術開發區前灣路218號
+Tel:86-532-86016016Fax:86-532-86016007
+____________________________________________________________________________________________________
+TERMSOFPAYMENT:60DAYSAMS
+TERMSOFSHIPMENT:FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTYUnit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0010 ADA4096-4ACPZ-R7 4570067453 1,500PC 2.892000 4,338.00
+______3_0_1_10_3_0_5_01________________8_0_7_9_42_9_7__________________________________________________________________
+Total: 1,500PC 4,338.00
+LessDepositPaid: 0.00
+NetTotal: 4,338.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出口事宜須知(編號EN-1102)isattached
+REF#AL0000037196,INV#90824626,BRAND:ADI,COUNTRYOFORIGIN:KOREA
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39WangKwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>世建发票3.pdf</t>
+        </is>
+      </c>
+      <c r="B484" t="n">
+        <v>3</v>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824632",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 30270.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824632",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 30270.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世健系統(香港)有限公司 InvoiceNo. :90824632
+Currency :USD
+IssuedBy :ShirleyHu
+Salesman :TONYGUO
+Date :09Aug2023
+CustomerCode :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIESCO
+COLIMITED LTD
+ROOMS3101-3105SINGGACOMMERCIALCENTRE NO218QIANWANROAD
+148CONNAUGHTROADWEST QINGDAOECONOMICANDTECHNOLOGICAL
+WESTERNDISTRICT,HongKong DEVELOPMENTZONE
+海信寬帶多媒體技術(香港)有限公司 QINGDAO
+Tel:852-25935622 QINGDAO,China
+PostalCode:266071
+青島海信寬帶多媒體技術有限公司
+青島經濟技術開發區前灣路218號
+Tel:86-532-86016016Fax:86-532-86016007
+____________________________________________________________________________________________________
+TERMSOFPAYMENT:60DAYSAMS
+TERMSOFSHIPMENT:FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTYUnit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0040 AD5679RBCPZ-2-RL7 4570067453 1,500PC 20.180000 30,270.00
+______3_0_1_11_3_0_4_01________________8_0_7_9_43_0_2__________________________________________________________________
+Total: 1,500PC 30,270.00
+LessDepositPaid: 0.00
+NetTotal: 30,270.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出口事宜須知(編號EN-1102)isattached
+REF#AL0000037196,INV#90824632,BRAND:ADI,COUNTRYOFORIGIN:SOUTH
+KOREA
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39WangKwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>世建发票3.pdf</t>
+        </is>
+      </c>
+      <c r="B485" t="n">
+        <v>4</v>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824629",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 5576.69,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824629",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 5576.69,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世健系統(香港)有限公司 InvoiceNo. :90824629
+Currency :USD
+IssuedBy :ShirleyHu
+Salesman :TONYGUO
+Date :09Aug2023
+CustomerCode :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIESCO
+COLIMITED LTD
+ROOMS3101-3105SINGGACOMMERCIALCENTRE NO218QIANWANROAD
+148CONNAUGHTROADWEST QINGDAOECONOMICANDTECHNOLOGICAL
+WESTERNDISTRICT,HongKong DEVELOPMENTZONE
+海信寬帶多媒體技術(香港)有限公司 QINGDAO
+Tel:852-25935622 QINGDAO,China
+PostalCode:266071
+青島海信寬帶多媒體技術有限公司
+青島經濟技術開發區前灣路218號
+Tel:86-532-86016016Fax:86-532-86016007
+____________________________________________________________________________________________________
+TERMSOFPAYMENT:60DAYSAMS
+TERMSOFSHIPMENT:FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTYUnit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0030 LTC3311SEV#PBF 4570066240 1,872PC 2.979000 5,576.69
+______3_0_1_11_1_5_8_01________________8_0_7_9_43_0_0__________________________________________________________________
+Total: 1,872PC 5,576.69
+LessDepositPaid: 0.00
+NetTotal: 5,576.69
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出口事宜須知(編號EN-1102)isattached
+REF#AL0000036955,INV#90824629,BRAND:ADI,COUNTRYOFORIGIN:SOUTH
+KOREA
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39WangKwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>世建发票3.pdf</t>
+        </is>
+      </c>
+      <c r="B486" t="n">
+        <v>5</v>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824628",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 873.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824628",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 873.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世健系統(香港)有限公司 InvoiceNo. :90824628
+Currency :USD
+IssuedBy :ShirleyHu
+Salesman :TONYGUO
+Date :09Aug2023
+CustomerCode :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIESCO
+COLIMITED LTD
+ROOMS3101-3105SINGGACOMMERCIALCENTRE NO218QIANWANROAD
+148CONNAUGHTROADWEST QINGDAOECONOMICANDTECHNOLOGICAL
+WESTERNDISTRICT,HongKong DEVELOPMENTZONE
+海信寬帶多媒體技術(香港)有限公司 QINGDAO
+Tel:852-25935622 QINGDAO,China
+PostalCode:266071
+青島海信寬帶多媒體技術有限公司
+青島經濟技術開發區前灣路218號
+Tel:86-532-86016016Fax:86-532-86016007
+____________________________________________________________________________________________________
+TERMSOFPAYMENT:60DAYSAMS
+TERMSOFSHIPMENT:FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTYUnit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0050 LTC3308AEV#TRMPBF 4570066645 500PC 1.746000 873.00
+______3_0_1_11_0_8_1_01________________8_0_7_9_42_9_9__________________________________________________________________
+Total: 500PC 873.00
+LessDepositPaid: 0.00
+NetTotal: 873.00
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出口事宜須知(編號EN-1102)isattached
+REF#AL0000037071,INV#90824628,BRAND:ADI,COUNTRYOFORIGIN:SOUTH
+KOREA
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39WangKwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>世建发票3.pdf</t>
+        </is>
+      </c>
+      <c r="B487" t="n">
+        <v>6</v>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824625",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 5104.5,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "90824625",
+    "Invoice Date": "09 Aug 2023",
+    "Currency": "USD",
+    "Amount": 5104.5,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO LIMITED",
+    "From": "Excelpoint Systems (H.K.) Limited",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t>ExcelpointSystems(H.K.)Limited Page :1/ 1
+世健系統(香港)有限公司 InvoiceNo. :90824625
+Currency :USD
+IssuedBy :ShirleyHu
+Salesman :TONYGUO
+Date :09Aug2023
+CustomerCode :6000004601
+____________________________________________________________________________________________________
+INVOICE
+____________________________________________________________________________________________________
+BILLTO: SOLDTO:
+HISENSEBROADBANDMULTIMEDIATECHNOLOGIES(HK) HISENSEBROADBANDMULTIMEDIATECHNOLOGIESCO
+COLIMITED LTD
+ROOMS3101-3105SINGGACOMMERCIALCENTRE NO218QIANWANROAD
+148CONNAUGHTROADWEST QINGDAOECONOMICANDTECHNOLOGICAL
+WESTERNDISTRICT,HongKong DEVELOPMENTZONE
+海信寬帶多媒體技術(香港)有限公司 QINGDAO
+Tel:852-25935622 QINGDAO,China
+PostalCode:266071
+青島海信寬帶多媒體技術有限公司
+青島經濟技術開發區前灣路218號
+Tel:86-532-86016016Fax:86-532-86016007
+____________________________________________________________________________________________________
+TERMSOFPAYMENT:60DAYSAMS
+TERMSOFSHIPMENT:FCAHONGKONG
+_____________________________________________________________________________________________________
+Item# Productcode PONo QTYUnit Unitprice Amount
+ExcelPointP/N DNNo
+CustomerP/N
+_____________________________________________________________________________________________________
+0010 ADN8834ACBZ-R7 4570065810 1,500PC 3.403000 5,104.50
+______3_0_1_01_1_8_3_01________________8_0_7_9_42_9_4__________________________________________________________________
+Total: 1,500PC 5,104.50
+LessDepositPaid: 0.00
+NetTotal: 5,104.50
+======================================================================================
+____________________________________________________________________________________________________
+ThisInvoiceisacomputerprintoutandnosignatureisrequired
+SHIPPINGMARKS:
+Remarks:
+出口事宜須知(編號EN-1102)isattached
+REF#AL0000036866,INV#90824625,BRAND:ADI,COUNTRYOFORIGIN:SINGAPORE
+____________________________________________________________________________________________________
+Address:3108,31/F,SkylineTower,39WangKwongRoad,,HongKong
+Phone:(852)2503-2212FAX:(852)2503-1558</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>WIN TREND XSCKD-SD-230818-09333.pdf</t>
+        </is>
+      </c>
+      <c r="B488" t="n">
+        <v>1</v>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230818-09333",
+    "Invoice Date": "2023-08-18",
+    "Currency": "USD",
+    "Amount": 1078.0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co., Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230818-09333",
+    "Invoice Date": "2023-08-18",
+    "Currency": "USD",
+    "Amount": 1078.0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co., Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>INVOICE
+Win Trend Electronic Technology Limited.
+6/F, EVERWIN CENTRE, NO.72 HUNG TO ROAD, KWUN TONG, KOWLOON, HONG KONG
+Invoice no.: XSCKD-SD-230818-09333
+Tel :Sally Siu 9623 7440 / Angie Kwan 9408 3888
+Bill to: Hisense Broadband Multimedia Technologies (HK) Co.,Ltd Date: 2023-08-18
+Attn. To: Shipping Terms
+Tel.: +86(0)532-80879676 / 18366214997 Payment Terms:月结60天
+Room 3101-3105, Singga Commercial Centre, 148 Connaught
+Add.: Sales: 孙志鹏
+Rd. West, Sai Ying Pun, HK
+QTY U/P AMT
+ITEM CSTM P/O NO. BRAND CSTM P/N DESCRIPTION
+PCS USD USD
+1 4570072564 CREDO/默升 3011105301 CFD50502-A0-ABXN 98 11.00 1078.00
+合计： 98 1078.00
+Beneficiary:Win Trend Electronic Technology Ltd.
+Bank Name:The Hong Kong and Shanghai Banking Corporation Ltd.
+Add.: No.1 Queen's Road Central, Hong Kong
+A/C No.: 848 533 097 838
+Swift Code:HSBCHKHHHKH
+送貨地址: 青旅思捷物流有限公司CYTS-SPIRIT LOGISTICS LIMITED
+香港荃灣橫窩仔街43-57號永得利中心六樓6/F, Ever Gain Centre, 43-57 Wang Wo Tsai Street, Tsuen Wan, N.T., Hong Kong
+TEL: 31522431 联系人： Mr. Key (阿仁)
+入仓单号： ZGD-506019 备注： 江门
+E. &amp; O. E.
+CONFIRM &amp; RECEIVED BY:</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>WIN TREND XSCKD-SD-230818-09333.pdf</t>
+        </is>
+      </c>
+      <c r="B489" t="n">
+        <v>2</v>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "非发票：可能是装货单、waybill或其他"
+}</t>
+        </is>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "非发票：可能是装货单、waybill或其他"
+}</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t>PACKING LIST
+Win Trend Electronic Technology Limited
+6/F, EVERWIN CENTRE, NO.72 HUNG TO ROAD, KWUN TONG, KOWLOON, HONG KONG
+Tel :Sally Siu 9623 7440 / Angie Kwan 9408 3888
+Bill to: Date: 2023-08-18
+Hisense Broadband Multimedia Technologies (HK) Co.,Ltd Invoice No. :XSCKD-SD-230818-09333
+Ship to: TEL: 31522431
+青旅思捷物流有限公司
+CYTS-SPIRIT LOGISTICS LIMITED
+Contact: Mr. Key (阿仁)
+香港荃灣橫窩仔街43-57號永得利中心六樓
+6/F, Ever Gain Centre, 43-57 Wang Wo Tsai Street, Tsuen Wan, N.T., Hong
+Kong
+N.W. G.W.
+QTY SIZE
+CTN No. PART No. CSTM PART No. PO NO. BRAND COO /CTN /CTN Remark
+(PCS) ( CM )
+KG KG
+CREDO/默
+1 CFD50502-A0-ABXN 3011105301 4570072564 KR 98 0.9 1.3 40X40X15 江门
+升
+合计： 98
+for and on behalf of for and on behalf of
+WIN TREND Electronic Technology Limited.
+Authorized Signatures Confirmed &amp; Received by</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>WIN TREND XSCKD-SD-230818-09341.pdf</t>
+        </is>
+      </c>
+      <c r="B490" t="n">
+        <v>1</v>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230818-09341",
+    "Invoice Date": "2023-08-18",
+    "Currency": "USD",
+    "Amount": 0.0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co.,Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230818-09341",
+    "Invoice Date": "2023-08-18",
+    "Currency": "USD",
+    "Amount": 0.0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co.,Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t>INVOICE
+Win Trend Electronic Technology Limited.
+6/F, EVERWIN CENTRE, NO.72 HUNG TO ROAD, KWUN TONG, KOWLOON, HONG KONG
+Invoice no.: XSCKD-SD-230818-09341
+Tel :Sally Siu 9623 7440 / Angie Kwan 9408 3888
+Bill to: Hisense Broadband Multimedia Technologies (HK) Co.,Ltd Date: 2023-08-18
+Attn. To: Shipping Terms:
+Tel.: +86(0)532-80879676 / 18366214997 Payment Terms: 月结60天
+Room 3101-3105, Singga Commercial Centre, 148 Connaught
+Add.: Sales: 孙志鹏
+Rd. West, Sai Ying Pun, HK
+QTY U/P AMT
+ITEM CSTM P/O NO. BRAND CSTM P/N DESCRIPTION
+PCS USD USD
+1 5010001959 CREDO/默升 3011105301 CFD50502-A0-ABXN 120 0.00 0.00
+合计： 120 0.00
+Beneficiary:Win Trend Electronic Technology Ltd.
+Bank Name:The Hong Kong and Shanghai Banking Corporation Ltd.
+Add.: No.1 Queen's Road Central, Hong Kong
+A/C No.: 848 533 097 838
+Swift Code:HSBCHKHHHKH
+送貨地址: 青旅思捷物流有限公司CYTS-SPIRIT LOGISTICS LIMITED
+香港荃灣橫窩仔街43-57號永得利中心六樓6/F, Ever Gain Centre, 43-57 Wang Wo Tsai Street, Tsuen Wan, N.T., Hong Kong
+TEL: 31522431 联系人： Mr. Key (阿仁)
+ZGD-506021 江门
+入仓单号： 备注：
+E. &amp; O. E.
+CONFIRM &amp; RECEIVED BY:</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>WIN TREND XSCKD-SD-230818-09341.pdf</t>
+        </is>
+      </c>
+      <c r="B491" t="n">
+        <v>2</v>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "非发票：可能是装货单、waybill或其他"
+}</t>
+        </is>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "非发票：可能是装货单、waybill或其他"
+}</t>
+        </is>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t>PACKING LIST
+Win Trend Electronic Technology Limited
+6/F, EVERWIN CENTRE, NO.72 HUNG TO ROAD, KWUN TONG, KOWLOON, HONG KONG
+Tel :Sally Siu 9623 7440 / Angie Kwan 9408 3888
+Bill to: Date: 2023-08-18
+Hisense Broadband Multimedia Technologies (HK) Co.,Ltd Invoice No. : XSCKD-SD-230818-09341
+Ship to: TEL: 31522431
+青旅思捷物流有限公司
+CYTS-SPIRIT LOGISTICS LIMITED
+Contact: Mr. Key (阿仁)
+香港荃灣橫窩仔街43-57號永得利中心六樓
+6/F, Ever Gain Centre, 43-57 Wang Wo Tsai Street, Tsuen Wan, N.T., Hong
+Kong
+N.W. G.W.
+QTY SIZE
+CTN No. PART No. CSTM PART No. PO NO. BRAND COO /CTN /CTN Remark
+(PCS) ( CM )
+KG KG
+CREDO/默
+1 CFD50502-A0-ABXN 3011105301 5010001959 TW,CN 120 0.7 1.4 40X40X15 江门
+升
+合计： 1 120 0.7 1.4
+for and on behalf of for and on behalf of
+WIN TREND Electronic Technology Limited.
+Authorized Signatures Confirmed &amp; Received by</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>WIN TREND XSCKD-SD-230907-09490.pdf</t>
+        </is>
+      </c>
+      <c r="B492" t="n">
+        <v>1</v>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "其他",
+    "Invoice No.": "",
+    "Invoice Date": "2023-09-07",
+    "Currency": "",
+    "Amount": 0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co.,Ltd",
+    "From": "WIN TREND Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "其他",
+    "Invoice No.": "",
+    "Invoice Date": "2023-09-07",
+    "Currency": "",
+    "Amount": 0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co.,Ltd",
+    "From": "WIN TREND Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t>PACKING
+G LIST
+胜达科
+WIN TREND TECHNOLOGY
+Win Trend ElectronicTechnology Limited
+6/F,EVERWINCENTRE,NO.72HUNGTOROAD,KWUNTONG,KOWLOON,HONGKONG
+Tel:Sally Siu 96237440/Angie Kwan 94083888
+Bill to:
+Date:
+2023-09-07
+Hisense Broadband Multimedia Technologies (HK) Co.,Ltd
+Invoice No.: XSCKD-SD-230907-09490
+Ship to:
+TEL:
+31522431
+青旅思捷物流有限公司
+CYTS-SPIRIT LOGISTICS LIMITED
+Contact:
+Mr.Key（阿仁）
+香港荃灣横商仔街43-57號永得利中心六楼
+6/F. Ever Gain Centre. 43-57 Wang Wo Tsai Street. Tsuen Wan. N.T..
+N.W.
+G.W.
+BRAND
+QTY
+SIZE
+CTN No.
+PART No.
+CSTM PART No.
+PO NO.
+COO
+/CTN
+/CTN
+(PCS)
+(CM）
+KG
+KG
+1
+MP2161GJ-Z
+3010074101
+/
+MPS/芯源
+CHINA
+6000
+0.5
+0.8
+24X23X14
+合计：
+1
+0.5
+0.8
+for and on behalf of
+for and on behalf of
+WIN TREND Electronic Technology Limited.
+Authorized Signatures
+Confirmed &amp; Received by</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>WIN TREND XSCKD-SD-230907-09490.pdf</t>
+        </is>
+      </c>
+      <c r="B493" t="n">
+        <v>2</v>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230907-09490",
+    "Invoice Date": "2023-09-07",
+    "Currency": "USD",
+    "Amount": 559.8,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co.,Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230907-09490",
+    "Invoice Date": "2023-09-07",
+    "Currency": "USD",
+    "Amount": 559.8,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co.,Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t>INVOICE
+WIN TREMD FECHBNO)IOGY
+Win Trend Electronic Technology Limited.
+6/F, EVERWIN CENTRE, NO.72 HUNG TO ROAD, KWUN TONG, KOWLOON, HONG KONG
+Invoice no.:
+XSCKD-SD-230907-09490
+Tel :Sally Siu 9623 7440 / Angie Kwan 9408 3888
+Bill to:
+Hisense Broadband Multimedia Technologies (HK) Co.,Ltd
+Date:
+2023-09-07
+Attn. To:
+Shipping
+Tel. :
++86 (0)532-80879676 / 18366214997
+Payment
+月结60天
+Room 3101-3105, Singga Commercial Centre,148 Connaught Rd.
+Add. :
+Sales:
+孙志鹏
+West, Sai Ying Pun, HK
+QTY
+d/n
+AMT
+ITEM
+CSTM P/0 NO.
+BRAND
+CSTM P/N
+DESCRIPTION
+PCS
+USD
+USD
+1
+MPS/芯源
+3010074101
+MP2161GJ-Z
+6000
+0.0933
+559.80
+Beneficiary:Win Trend Electronic Technology Ltd.
+Bank Name:The Hong Kong and Shanghai Banking Corporation Ltd.
+Add.: No.1 Queen' s Road Central, Hong Kong
+A/C No.:848533097838
+Swift Code:HSBCHKHHHKH
+送货地址：
+青旅思捷物流有限公司CYTS-SPIRIT LOGISTICSLIMITED
+香港基灣横仔街43-57號永得利中心六樓6/F，Ever Gain Centre，43-57Wang Wo Tsai Street，Tsuen Wan，N.T.，Hong Kong
+TEL:
+31522431
+联系人：
+Mr.Key (阿仁)
+入仓单号：
+NA
+备注：
+青岛
+E.&amp;O.E.
+CONFIRM &amp; RECEIVED BY:</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>XSCKD-SD-230818-09332 INV-青岛.pdf</t>
+        </is>
+      </c>
+      <c r="B494" t="n">
+        <v>1</v>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230818-09332",
+    "Invoice Date": "2023-08-18",
+    "Currency": "USD",
+    "Amount": 5170.0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co., Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "XSCKD-SD-230818-09332",
+    "Invoice Date": "2023-08-18",
+    "Currency": "USD",
+    "Amount": 5170.0,
+    "Bill To": "Hisense Broadband Multimedia Technologies (HK) Co., Ltd",
+    "From": "Win Trend Electronic Technology Limited"
+}</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>INVOICE
+Win Trend Electronic Technology Limited.
+6/F, EVERWIN CENTRE, NO.72 HUNG TO ROAD, KWUN TONG, KOWLOON, HONG KONG
+Invoice no.: XSCKD-SD-230818-09332
+Tel :Sally Siu 9623 7440 / Angie Kwan 9408 3888
+Bill to: Hisense Broadband Multimedia Technologies (HK) Co.,Ltd Date: 2023-08-18
+Attn. To: Shipping Terms:
+Tel.: +86(0)532-80879676 / 18366214997 Payment Terms: 月结60天
+Room 3101-3105, Singga Commercial Centre, 148 Connaught
+Add.: Sales: 孙志鹏
+Rd. West, Sai Ying Pun, HK
+QTY U/P AMT
+ITEM CSTM P/O NO. BRAND CSTM P/N DESCRIPTION
+PCS USD USD
+1 4570072564 CREDO/默升 3011105301 CFD50502-A0-ABXN 470 11.00 5170.00
+合计： 470 5170.00
+Beneficiary:Win Trend Electronic Technology Ltd.
+Bank Name:The Hong Kong and Shanghai Banking Corporation Ltd.
+Add.: No.1 Queen's Road Central, Hong Kong
+A/C No.: 848 533 097 838
+Swift Code:HSBCHKHHHKH
+送貨地址: 青旅思捷物流有限公司CYTS-SPIRIT LOGISTICS LIMITED
+香港荃灣橫窩仔街43-57號永得利中心六樓6/F, Ever Gain Centre, 43-57 Wang Wo Tsai Street, Tsuen Wan, N.T., Hong Kong
+TEL: 31522431 联系人： Mr. Key (阿仁)
+入仓单号： NA 备注： 青岛
+E. &amp; O. E.
+CONFIRM &amp; RECEIVED BY:</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>HK00213203.pdf</t>
+        </is>
+      </c>
+      <c r="B495" t="n">
+        <v>1</v>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "HK00213203",
+    "Invoice Date": "2023/4/13",
+    "Currency": "USD",
+    "Amount": 27000.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO., LTD.",
+    "From": "HITACHI HIGH-TECH HONG KONG LTD",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "HK00213203",
+    "Invoice Date": "2023/4/13",
+    "Currency": "USD",
+    "Amount": 27000.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO., LTD.",
+    "From": "HITACHI HIGH-TECH HONG KONG LTD",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>Hitachi High-Tech Hong Kong Ltd.
+8/F, Building 20E, Phase 3, Hong Kong Science Park,
+Pak Shek Kok, N.T., Hong Kong
+TEL: 852-2737-4700
+FAX: 852-2370-7255
+Invoice
+Bill To: PAGE 1/1
+Purchasing Departmet Invoice No.: HK00213203
+HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO.,LTD. Invoice Date : 2023/4/13
+ROOMS 3010-3105 SINGGA COMMERCIAL CENTRE Inco Terms : FCA JAPAN
+148 CONNAUGHT ROAD WEST HONG KONG Terms Of Payment : T/T 60 DAYS MONTYLY
+Shipped Per : DHL
+Ship To : Shipment date: 2023/4/13
+Loading Port : TOKYO
+CYTS-SPIRIT LOGISTICS LIMITED Discharge Port : HONG KONG
+Eternity Warehouse 6/F, Ever Gain Centre, 43-57 Wang Wo Tsai Street, Vendor Code: 5001060
+Tsuen Wan, N.T.. HONGKONG
+boyim@cyts-spirit.com
+Item Cust. PO No. Description Part NO. Quantity Unit Price Amount
+(PCS) (USD) (USD)
+1 4510070120 4431004801 1-P7175-01-R00 100,000 0.27 27,000.00
+Total : 100,000 27,000.00
+Packing list
+COUNTRY Gross
+OF ORIGIN Quantity(PCS) Carton Net Weight(KGS) Weight(KGS) CBM(M3)
+JAPAN 4431004801 50,000 2-1 0.10 3.30 0.017204
+4431004801 50,000 2-2 0.10 3.30 0.017204
+Total: 100,000 2 0.20 6.60 0.034
+Remarks:
+入仓号: ZGD-505007 (广东宽带多媒体货物)
+Remit to : MUFG BANK LTD HONG KONG BRANCH
+Account Name : HITACHI HIGH-TECH HONG KONG LTD
+Account No : 047-821-85806018194
+Swift Code : BOTKHKHH
+for Hitachi High-Tech Hong Kong Ltd.
+Authorized Signature</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>HK00214688.pdf</t>
+        </is>
+      </c>
+      <c r="B496" t="n">
+        <v>1</v>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "HK00214688",
+    "Invoice Date": "2023/7/7",
+    "Currency": "USD",
+    "Amount": 4800.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO., LTD.",
+    "From": "HITACHI HIGH-TECH HONG KONG LTD",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "HK00214688",
+    "Invoice Date": "2023/7/7",
+    "Currency": "USD",
+    "Amount": 4800.0,
+    "Bill To": "HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO., LTD.",
+    "From": "HITACHI HIGH-TECH HONG KONG LTD",
+    "page": "1/1"
+}</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>Hitachi High-Tech Hong Kong Ltd.
+8/F, Building 20E, Phase 3, Hong Kong Science Park,
+Pak Shek Kok, N.T., Hong Kong
+TEL: 852-2737-4700
+FAX: 852-2370-7255
+Invoice
+Bill To: PAGE 1/1
+Purchasing Departmet Invoice No.: HK00214688
+HISENSE BROADBAND MULTIMEDIA TECHNOLOGIES (HK) CO.,LTD. Invoice Date : 2023/7/7
+ROOMS 3010-3105 SINGGA COMMERCIAL CENTRE Inco Terms : FCA JAPAN
+148 CONNAUGHT ROAD WEST HONG KONG Terms Of Payment : T/T 60 DAYS MONTYLY
+Shipped Per : DHL
+Ship To : Shipment date: 2023/7/7
+Loading Port : TOKYO
+CYTS-SPIRIT LOGISTICS LIMITED Discharge Port : HONG KONG
+Eternity Warehouse 6/F, Ever Gain Centre, 43-57 Wang Wo Tsai Street, Vendor Code: 5001060
+Tsuen Wan, N.T.. HONGKONG
+boyim@cyts-spirit.com
+Item Cust. PO No. Description Part NO. Quantity Unit Price Amount
+(PCS) (USD) (USD)
+1 4570071385 KSHH018XCA 4501003801 1,000 4.80 4,800.00
+Total : 1,000 4,800.00
+Packing list
+COUNTRY Gross
+OF ORIGIN Quantity(PCS) Carton Net Weight(KGS) Weight(KGS) CBM(M3)
+JAPAN KSHH018XCA 1,000 1-1 0.05 0.70 0.01
+Total: 1,000 1 0.05 0.70 0.010
+Remarks:
+Remit to : MUFG BANK LTD HONG KONG BRANCH
+Account Name : HITACHI HIGH-TECH HONG KONG LTD
+Account No : 047-821-85806018194
+Swift Code : BOTKHKHH
+for Hitachi High-Tech Hong Kong Ltd.
+Authorized Signature</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>MISSION 5970023769.pdf</t>
+        </is>
+      </c>
+      <c r="B497" t="n">
+        <v>1</v>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "F230726000015",
+    "Invoice Date": "2023-07-26",
+    "Currency": "",
+    "Amount": 0,
+    "Bill To": "Hisense broadband multimedia technologies (HK) CO., Ltd",
+    "From": "Mission Electronics International Limited"
+}</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>{
+    "Doc Type": "Invoice",
+    "Invoice No.": "F230726000015",
+    "Invoice Date": "2023-07-26",
+    "Currency": "",
+    "Amount": 0,
+    "Bill To": "Hisense broadband multimedia technologies (HK) CO., Ltd",
+    "From": "Mission Electronics International Limited"
+}</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>美盛電子國際有限公司
+MISSION ELECTRONICSINTERNATIONAL LIMITED
+Webite:www.mission-io.com
+General line:((00852)27582283Fax:(00852)31051139
+美盛
+盛Address:香港九龍九龍灣宏開道20號杨耀崧第八工業大厦9樓E室
+NOISSIW
+Flat E,9/F,Yeung Yiu Chung (No.8) Industrial Building,No.20 Wang Hoi Road, Kowloon Bay,Kowloon
+57023272
+PACKINGLIST
+Customer:Hisense broadband multimedia technologies (HK) CO.,Ltd
+P.O.No.:5970023769
+InvoiceNo.:F230726000015
+PaymentTerm:发货单出货后30天付款(NET30)
+InvoiceDate:2023-07-26
+ShipVia:
+BillTo:Hisense broadbandmultimedia technologies(HK) CO.,Ltd
+ShipTo:CYTS-SPIRITLOGISTICS,LTD
+Room 3101-3105, Singga Commercial Centre, 148 Conaught R d.
+6/F,43-57.Wang Wo Tsai Street, Ever Gain centre ,Tsuen wan,
+West, Sai Ying Pun, HK
+NT,HONG KONG
+Attn:蔺艳莉
+Attn:BO YIM
+Tel:15684730865
+Tel:31522507
+数量
+重量
+尺寸
+产地
+行号
+客户料号Cusr
+规格型号
+DC
+Brand
+QTY
+Weight
+Dimension
+Country of
+LOT NO.
+CTN#
+Internalpart No.
+Part No.
+年份
+品牌
+(pcs)
+(KG)
+(cm)
+origin
+NW:2.3
+3011093801
+INA216A3YFFT
+750
+60*24*24
+2325
+T1
+1
+3431356CL3
+GW:3.7
+3011093801
+INA216A3YFFT
+1500
+2318
+Il.
+3304605CL3
+INA216A3YFFT
+500
+2318
+TI
+3011093801
+3304608CL3
+3011093801
+INA216A3YFFT
+2500
+2318
+T
+3304607CL3
+3011093801
+INA216A3YFFT
+500
+2318
+T
+3304606CL3
+3011093801
+INA216A3YFFT
+250
+2318
+T
+3304609CL3
+NW:1.2
+3011089901
+TPS62480RNCT
+6000
+42*15*43
+2141
+TI
+2141
+2
+GW:2.0
+3011089901
+3000
+2150
+2150
+TPS62480RNCT
+12000
+NW:2.8
+3
+3011089901
+TPS62480RNCT
+40*30*40
+2150
+T1
+2150
+GW:4.3
+3000
+2204
+TI
+3011089901
+TPS62480RNCT
+2204
+3011089901
+TPS62480RNCT
+6000
+2226
+TI
+2226
+Total:
+3
+Cartons
+36000 PCS
+NW: 6.3 KG ; GW: 10.0 KG
+Note:
+1.Purchase Order Number must be quoted on all documents to facilitate payment.
+2.No Cancellation ,No Return ,No Reschedule (except for Electronic Failure).
+3.Any complaints against this invoice must be notified to the company within 7 days of data hereof.
+4.We are not responsible for any banking charges outside ShenZhen The Payment received in our
+account must be the same as the amount we invoiced.
+For and on behalf of
+Confirmed and received by
+Mission ElectronicsInternational Limited
+Viki欧阳桃
+英盛
+请签章
+客子国際
+有限公司
+Customer Chop and Signature
+Authorized Signature</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>